<commit_message>
rev.1.001: adding PCB board file and Gerber file for invertor 24-380V
</commit_message>
<xml_diff>
--- a/Docs/BOM for invertor 24-380V.xlsx
+++ b/Docs/BOM for invertor 24-380V.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ilya\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Invertor\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="241">
   <si>
     <t>Comment</t>
   </si>
@@ -107,9 +107,6 @@
     <t>C29</t>
   </si>
   <si>
-    <t>470 μF</t>
-  </si>
-  <si>
     <t>C30, C31, C32, C33</t>
   </si>
   <si>
@@ -512,15 +509,9 @@
     <t>VT14, VT15</t>
   </si>
   <si>
-    <t>"Вход +24В"</t>
-  </si>
-  <si>
     <t>7461383</t>
   </si>
   <si>
-    <t>"Temp №1"</t>
-  </si>
-  <si>
     <t>WF-02</t>
   </si>
   <si>
@@ -729,13 +720,40 @@
   </si>
   <si>
     <t>Итог:</t>
+  </si>
+  <si>
+    <t>Разъем</t>
+  </si>
+  <si>
+    <t>X7</t>
+  </si>
+  <si>
+    <t>X977B02</t>
+  </si>
+  <si>
+    <t>https://www.chipdip.ru/product/x977b02</t>
+  </si>
+  <si>
+    <t>680 μF</t>
+  </si>
+  <si>
+    <t>220k</t>
+  </si>
+  <si>
+    <t>R83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC2512JK-07150KL </t>
+  </si>
+  <si>
+    <t>http://www.electronshik.ru/item/rc2512jk-07150kl-1133442</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -759,6 +777,13 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="10">
@@ -865,32 +890,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -909,17 +912,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -950,12 +942,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -964,34 +989,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1012,12 +1019,51 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -1301,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,1788 +1364,1824 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>168</v>
+      <c r="F1" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="21">
         <v>5</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="22">
         <v>0.28000000000000003</v>
       </c>
-      <c r="G2" s="14">
+      <c r="G2" s="22">
         <f>F2*E2</f>
         <v>1.4000000000000001</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>171</v>
+      <c r="H2" s="33" t="s">
+        <v>168</v>
       </c>
       <c r="I2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="6" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="3">
         <v>16</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="8">
         <v>68</v>
       </c>
-      <c r="G3" s="14">
-        <f t="shared" ref="G3:G61" si="0">F3*E3</f>
+      <c r="G3" s="8">
+        <f t="shared" ref="G3:G59" si="0">F3*E3</f>
         <v>1088</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>172</v>
+      <c r="H3" s="34" t="s">
+        <v>169</v>
       </c>
       <c r="I3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="6" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="3">
         <v>12</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="8">
         <v>0.37</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="8">
         <f t="shared" si="0"/>
         <v>4.4399999999999995</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>173</v>
+      <c r="H4" s="34" t="s">
+        <v>170</v>
       </c>
       <c r="I4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="3">
         <v>5</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="8">
         <v>0.25</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="8">
         <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>174</v>
+      <c r="H5" s="34" t="s">
+        <v>171</v>
       </c>
       <c r="I5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="6" t="s">
         <v>21</v>
       </c>
       <c r="E6" s="3">
         <v>3</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="8">
         <v>0.68</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="8">
         <f t="shared" si="0"/>
         <v>2.04</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>175</v>
+      <c r="H6" s="34" t="s">
+        <v>172</v>
       </c>
       <c r="I6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="6" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="3">
         <v>6</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="8">
         <v>22</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="8">
         <f t="shared" si="0"/>
         <v>132</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="I7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="I7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>178</v>
+      <c r="D8" s="6" t="s">
+        <v>175</v>
       </c>
       <c r="E8" s="3">
         <v>1</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="8">
         <v>0.66</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="8">
         <f t="shared" si="0"/>
         <v>0.66</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>177</v>
+      <c r="H8" s="34" t="s">
+        <v>174</v>
       </c>
       <c r="I8" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="C9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>30</v>
       </c>
       <c r="E9" s="3">
         <v>4</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="8">
         <v>234</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="8">
         <f t="shared" si="0"/>
         <v>936</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>180</v>
+      <c r="H9" s="34" t="s">
+        <v>177</v>
       </c>
       <c r="I9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>33</v>
+      <c r="D10" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="E10" s="3">
         <v>6</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="8">
         <v>6.7</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="8">
         <f t="shared" si="0"/>
         <v>40.200000000000003</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>181</v>
+      <c r="H10" s="34" t="s">
+        <v>178</v>
       </c>
       <c r="I10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>34</v>
+      <c r="B11" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>35</v>
+      <c r="D11" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="E11" s="3">
         <v>4</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="8">
         <v>10</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="8">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>182</v>
+      <c r="H11" s="34" t="s">
+        <v>179</v>
       </c>
       <c r="I11" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>38</v>
+      <c r="D12" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="E12" s="3">
         <v>2</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="8">
         <v>0.28000000000000003</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="8">
         <f t="shared" si="0"/>
         <v>0.56000000000000005</v>
       </c>
-      <c r="H12" s="6" t="s">
-        <v>183</v>
+      <c r="H12" s="34" t="s">
+        <v>180</v>
       </c>
       <c r="I12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="12" t="s">
-        <v>41</v>
+      <c r="D13" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="E13" s="3">
         <v>4</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="8">
         <v>0.3</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="8">
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
-      <c r="H13" s="6" t="s">
-        <v>184</v>
+      <c r="H13" s="34" t="s">
+        <v>181</v>
       </c>
       <c r="I13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="C14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>45</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="8">
         <v>7.1</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="8">
         <f t="shared" si="0"/>
         <v>7.1</v>
       </c>
-      <c r="H14" s="6" t="s">
-        <v>185</v>
+      <c r="H14" s="34" t="s">
+        <v>182</v>
       </c>
       <c r="I14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="12" t="s">
-        <v>46</v>
+      <c r="B15" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="12" t="s">
-        <v>47</v>
+      <c r="D15" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="8">
         <v>1.6</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="8">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>186</v>
+      <c r="H15" s="34" t="s">
+        <v>183</v>
       </c>
       <c r="I15" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="C16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>51</v>
       </c>
       <c r="E16" s="3">
         <v>5</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="8">
         <v>22.4</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="8">
         <f t="shared" si="0"/>
         <v>112</v>
       </c>
-      <c r="H16" s="6" t="s">
-        <v>187</v>
+      <c r="H16" s="34" t="s">
+        <v>184</v>
       </c>
       <c r="I16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="C17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>53</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>54</v>
       </c>
       <c r="E17" s="3">
         <v>2</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="8">
         <v>15</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="8">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="H17" s="6" t="s">
-        <v>188</v>
+      <c r="H17" s="34" t="s">
+        <v>185</v>
       </c>
       <c r="I17" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="C18" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>55</v>
+      <c r="D18" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="E18" s="3">
         <v>2</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="8">
         <v>18.2</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="8">
         <f t="shared" si="0"/>
         <v>36.4</v>
       </c>
-      <c r="H18" s="6" t="s">
-        <v>189</v>
+      <c r="H18" s="34" t="s">
+        <v>186</v>
       </c>
       <c r="I18" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="C19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>58</v>
+      <c r="D19" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="E19" s="3">
         <v>2</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="8">
         <v>197</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="8">
         <f t="shared" si="0"/>
         <v>394</v>
       </c>
-      <c r="H19" s="6" t="s">
-        <v>190</v>
+      <c r="H19" s="34" t="s">
+        <v>187</v>
       </c>
       <c r="I19" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="C20" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>61</v>
+      <c r="D20" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="E20" s="3">
         <v>2</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="8">
         <v>96</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="8">
         <f t="shared" si="0"/>
         <v>192</v>
       </c>
-      <c r="H20" s="6" t="s">
-        <v>191</v>
+      <c r="H20" s="34" t="s">
+        <v>188</v>
       </c>
       <c r="I20" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="C21" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>64</v>
+      <c r="D21" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="E21" s="3">
         <v>1</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="8">
         <v>12.8</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="8">
         <f t="shared" si="0"/>
         <v>12.8</v>
       </c>
-      <c r="H21" s="6" t="s">
-        <v>192</v>
+      <c r="H21" s="34" t="s">
+        <v>189</v>
       </c>
       <c r="I21" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="C22" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>67</v>
+      <c r="D22" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="E22" s="3">
         <v>1</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22" s="8">
         <v>240</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22" s="8">
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
-      <c r="H22" s="6" t="s">
-        <v>193</v>
+      <c r="H22" s="34" t="s">
+        <v>190</v>
       </c>
       <c r="I22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>71</v>
-      </c>
       <c r="C23" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>70</v>
+        <v>59</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="E23" s="3">
         <v>1</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="8">
         <v>87.5</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="8">
         <f t="shared" si="0"/>
         <v>87.5</v>
       </c>
-      <c r="H23" s="6" t="s">
-        <v>194</v>
+      <c r="H23" s="34" t="s">
+        <v>191</v>
       </c>
       <c r="I23" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="C24" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="6" t="s">
         <v>74</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>75</v>
       </c>
       <c r="E24" s="3">
         <v>1</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="8">
         <v>1.5</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="8">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="H24" s="6" t="s">
-        <v>195</v>
+      <c r="H24" s="34" t="s">
+        <v>192</v>
       </c>
       <c r="I24" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="C25" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="D25" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>79</v>
       </c>
       <c r="E25" s="3">
         <v>1</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F25" s="8">
         <v>220.41</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="8">
         <f t="shared" si="0"/>
         <v>220.41</v>
       </c>
-      <c r="H25" s="6" t="s">
-        <v>233</v>
+      <c r="H25" s="34" t="s">
+        <v>230</v>
       </c>
       <c r="I25" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="C26" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="D26" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>83</v>
       </c>
       <c r="E26" s="3">
         <v>2</v>
       </c>
-      <c r="F26" s="14">
+      <c r="F26" s="8">
         <v>36</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="8">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="H26" s="6" t="s">
-        <v>196</v>
+      <c r="H26" s="34" t="s">
+        <v>193</v>
       </c>
       <c r="I26" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>85</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>86</v>
+      <c r="D27" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="E27" s="3">
         <v>1</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F27" s="8">
         <v>0.12</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="8">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
-      <c r="H27" s="6" t="s">
-        <v>197</v>
+      <c r="H27" s="34" t="s">
+        <v>194</v>
       </c>
       <c r="I27" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>87</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>88</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="12" t="s">
-        <v>89</v>
+      <c r="D28" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="E28" s="3">
         <v>1</v>
       </c>
-      <c r="F28" s="14">
+      <c r="F28" s="8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="8">
         <f t="shared" si="0"/>
         <v>0.14000000000000001</v>
       </c>
-      <c r="H28" s="6" t="s">
-        <v>198</v>
+      <c r="H28" s="34" t="s">
+        <v>195</v>
       </c>
       <c r="I28" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>91</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="12" t="s">
-        <v>92</v>
+      <c r="D29" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="E29" s="3">
         <v>9</v>
       </c>
-      <c r="F29" s="14">
+      <c r="F29" s="8">
         <v>0.1</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="8">
         <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
-      <c r="H29" s="6" t="s">
-        <v>199</v>
+      <c r="H29" s="34" t="s">
+        <v>196</v>
       </c>
       <c r="I29" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>94</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="12" t="s">
-        <v>95</v>
+      <c r="D30" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="E30" s="3">
         <v>6</v>
       </c>
-      <c r="F30" s="14">
+      <c r="F30" s="8">
         <v>0.13</v>
       </c>
-      <c r="G30" s="14">
+      <c r="G30" s="8">
         <f t="shared" si="0"/>
         <v>0.78</v>
       </c>
-      <c r="H30" s="6" t="s">
-        <v>200</v>
+      <c r="H30" s="34" t="s">
+        <v>197</v>
       </c>
       <c r="I30" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>96</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>97</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="12" t="s">
-        <v>98</v>
+      <c r="D31" s="6" t="s">
+        <v>97</v>
       </c>
       <c r="E31" s="3">
         <v>1</v>
       </c>
-      <c r="F31" s="14">
+      <c r="F31" s="8">
         <v>0.15</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="8">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="H31" s="6" t="s">
-        <v>201</v>
+      <c r="H31" s="34" t="s">
+        <v>198</v>
       </c>
       <c r="I31" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>100</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>101</v>
+      <c r="D32" s="6" t="s">
+        <v>100</v>
       </c>
       <c r="E32" s="3">
         <v>2</v>
       </c>
-      <c r="F32" s="14">
+      <c r="F32" s="8">
         <v>0.12</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="8">
         <f t="shared" si="0"/>
         <v>0.24</v>
       </c>
-      <c r="H32" s="6" t="s">
-        <v>202</v>
+      <c r="H32" s="34" t="s">
+        <v>199</v>
       </c>
       <c r="I32" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>103</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="12" t="s">
-        <v>104</v>
+      <c r="D33" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="E33" s="3">
         <v>10</v>
       </c>
-      <c r="F33" s="14">
+      <c r="F33" s="8">
         <v>0.1</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="6" t="s">
-        <v>203</v>
+      <c r="H33" s="34" t="s">
+        <v>200</v>
       </c>
       <c r="I33" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>105</v>
+      <c r="A34" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="12" t="s">
-        <v>106</v>
+      <c r="D34" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="E34" s="3">
         <v>4</v>
       </c>
-      <c r="F34" s="14">
+      <c r="F34" s="8">
         <v>0.12</v>
       </c>
-      <c r="G34" s="14">
+      <c r="G34" s="8">
         <f t="shared" si="0"/>
         <v>0.48</v>
       </c>
-      <c r="H34" s="6" t="s">
-        <v>204</v>
+      <c r="H34" s="34" t="s">
+        <v>201</v>
       </c>
       <c r="I34" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>108</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="12" t="s">
-        <v>205</v>
+      <c r="D35" s="6" t="s">
+        <v>202</v>
       </c>
       <c r="E35" s="3">
         <v>2</v>
       </c>
-      <c r="F35" s="14">
+      <c r="F35" s="8">
         <v>0.11</v>
       </c>
-      <c r="G35" s="14">
+      <c r="G35" s="8">
         <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
-      <c r="H35" s="6" t="s">
-        <v>206</v>
+      <c r="H35" s="34" t="s">
+        <v>203</v>
       </c>
       <c r="I35" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>110</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="12" t="s">
-        <v>111</v>
+      <c r="D36" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="E36" s="3">
         <v>1</v>
       </c>
-      <c r="F36" s="14">
+      <c r="F36" s="8">
         <v>0.09</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G36" s="8">
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
-      <c r="H36" s="6" t="s">
-        <v>207</v>
+      <c r="H36" s="34" t="s">
+        <v>204</v>
       </c>
       <c r="I36" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>112</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>113</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="12" t="s">
-        <v>208</v>
+      <c r="D37" s="6" t="s">
+        <v>205</v>
       </c>
       <c r="E37" s="3">
         <v>12</v>
       </c>
-      <c r="F37" s="14">
+      <c r="F37" s="8">
         <v>0.11</v>
       </c>
-      <c r="G37" s="14">
+      <c r="G37" s="8">
         <f t="shared" si="0"/>
         <v>1.32</v>
       </c>
-      <c r="H37" s="6" t="s">
-        <v>209</v>
+      <c r="H37" s="34" t="s">
+        <v>206</v>
       </c>
       <c r="I37" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>114</v>
+      <c r="A38" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="12" t="s">
-        <v>115</v>
+      <c r="D38" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="E38" s="3">
         <v>21</v>
       </c>
-      <c r="F38" s="14">
+      <c r="F38" s="8">
         <v>0.11</v>
       </c>
-      <c r="G38" s="14">
+      <c r="G38" s="8">
         <f t="shared" si="0"/>
         <v>2.31</v>
       </c>
-      <c r="H38" s="6" t="s">
-        <v>210</v>
+      <c r="H38" s="34" t="s">
+        <v>207</v>
       </c>
       <c r="I38" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B39" s="12" t="s">
+      <c r="A39" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>116</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>117</v>
       </c>
       <c r="E39" s="3">
         <v>3</v>
       </c>
-      <c r="F39" s="14">
+      <c r="F39" s="8">
         <v>43.6</v>
       </c>
-      <c r="G39" s="14">
+      <c r="G39" s="8">
         <f t="shared" si="0"/>
         <v>130.80000000000001</v>
       </c>
-      <c r="H39" s="6" t="s">
-        <v>211</v>
+      <c r="H39" s="34" t="s">
+        <v>208</v>
       </c>
       <c r="I39" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40" s="6" t="s">
         <v>118</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>119</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D40" s="12" t="s">
-        <v>120</v>
+      <c r="D40" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="E40" s="3">
         <v>1</v>
       </c>
-      <c r="F40" s="14">
+      <c r="F40" s="8">
         <v>0.12</v>
       </c>
-      <c r="G40" s="14">
+      <c r="G40" s="8">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
-      <c r="H40" s="6" t="s">
-        <v>212</v>
+      <c r="H40" s="34" t="s">
+        <v>209</v>
       </c>
       <c r="I40" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B41" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>122</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D41" s="12" t="s">
-        <v>123</v>
+      <c r="D41" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="E41" s="3">
         <v>1</v>
       </c>
-      <c r="F41" s="14">
+      <c r="F41" s="8">
         <v>0.12</v>
       </c>
-      <c r="G41" s="14">
+      <c r="G41" s="8">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
-      <c r="H41" s="6" t="s">
-        <v>213</v>
+      <c r="H41" s="34" t="s">
+        <v>210</v>
       </c>
       <c r="I41" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>124</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>125</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D42" s="12" t="s">
-        <v>126</v>
+      <c r="D42" s="6" t="s">
+        <v>125</v>
       </c>
       <c r="E42" s="3">
         <v>7</v>
       </c>
-      <c r="F42" s="14">
+      <c r="F42" s="8">
         <v>0.13</v>
       </c>
-      <c r="G42" s="14">
+      <c r="G42" s="8">
         <f t="shared" si="0"/>
         <v>0.91</v>
       </c>
-      <c r="H42" s="6" t="s">
-        <v>214</v>
+      <c r="H42" s="34" t="s">
+        <v>211</v>
       </c>
       <c r="I42" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="B43" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="C43" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="E43" s="30">
+        <v>1</v>
+      </c>
+      <c r="F43" s="31">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G43" s="31">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H43" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="I43" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="C44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E44" s="3">
+        <v>2</v>
+      </c>
+      <c r="F44" s="8">
+        <v>332.9</v>
+      </c>
+      <c r="G44" s="8">
+        <f>F44*E44</f>
+        <v>665.8</v>
+      </c>
+      <c r="H44" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="I44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="E43" s="3">
-        <v>2</v>
-      </c>
-      <c r="F43" s="14">
-        <v>332.9</v>
-      </c>
-      <c r="G43" s="14">
-        <f t="shared" si="0"/>
-        <v>665.8</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="I43" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="B45" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="C45" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="E44" s="3">
-        <v>1</v>
-      </c>
-      <c r="F44" s="14">
-        <v>9.4</v>
-      </c>
-      <c r="G44" s="14">
-        <f t="shared" si="0"/>
-        <v>9.4</v>
-      </c>
-      <c r="H44" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="I44" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>132</v>
+      <c r="D45" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="E45" s="3">
         <v>1</v>
       </c>
-      <c r="F45" s="14">
+      <c r="F45" s="8">
+        <v>9.4</v>
+      </c>
+      <c r="G45" s="8">
+        <f>F45*E45</f>
+        <v>9.4</v>
+      </c>
+      <c r="H45" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="I45" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E46" s="3">
+        <v>1</v>
+      </c>
+      <c r="F46" s="8">
         <v>2.1</v>
       </c>
-      <c r="G45" s="14">
-        <f t="shared" si="0"/>
+      <c r="G46" s="8">
+        <f>F46*E46</f>
         <v>2.1</v>
       </c>
-      <c r="H45" s="6" t="s">
+      <c r="H46" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="I46" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E47" s="3">
+        <v>16</v>
+      </c>
+      <c r="F47" s="8">
+        <v>16</v>
+      </c>
+      <c r="G47" s="8">
+        <f>F47*E47</f>
+        <v>256</v>
+      </c>
+      <c r="H47" s="34" t="s">
+        <v>214</v>
+      </c>
+      <c r="I47" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E48" s="3">
+        <v>4</v>
+      </c>
+      <c r="F48" s="8">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G48" s="8">
+        <f>F48*E48</f>
+        <v>17.600000000000001</v>
+      </c>
+      <c r="H48" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="I48" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E49" s="3">
+        <v>12</v>
+      </c>
+      <c r="F49" s="8">
+        <v>5.9</v>
+      </c>
+      <c r="G49" s="8">
+        <f>F49*E49</f>
+        <v>70.800000000000011</v>
+      </c>
+      <c r="H49" s="34" t="s">
         <v>216</v>
       </c>
-      <c r="I45" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="E46" s="3">
-        <v>16</v>
-      </c>
-      <c r="F46" s="14">
-        <v>16</v>
-      </c>
-      <c r="G46" s="14">
-        <f t="shared" si="0"/>
-        <v>256</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="I46" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="E47" s="3">
+      <c r="I49" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E50" s="3">
+        <v>8</v>
+      </c>
+      <c r="F50" s="8">
+        <v>45</v>
+      </c>
+      <c r="G50" s="8">
+        <f>F50*E50</f>
+        <v>360</v>
+      </c>
+      <c r="H50" s="34" t="s">
+        <v>218</v>
+      </c>
+      <c r="I50" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E51" s="3">
+        <v>1</v>
+      </c>
+      <c r="F51" s="8">
+        <v>7.2</v>
+      </c>
+      <c r="G51" s="8">
+        <f>F51*E51</f>
+        <v>7.2</v>
+      </c>
+      <c r="H51" s="34" t="s">
+        <v>219</v>
+      </c>
+      <c r="I51" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E52" s="3">
+        <v>2</v>
+      </c>
+      <c r="F52" s="8">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="G52" s="8">
+        <f>F52*E52</f>
+        <v>18.600000000000001</v>
+      </c>
+      <c r="H52" s="34" t="s">
+        <v>220</v>
+      </c>
+      <c r="I52" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1</v>
+      </c>
+      <c r="F53" s="8">
         <v>4</v>
       </c>
-      <c r="F47" s="14">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="G47" s="14">
-        <f t="shared" si="0"/>
-        <v>17.600000000000001</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="I47" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="E48" s="3">
+      <c r="G53" s="8">
+        <f>F53*E53</f>
+        <v>4</v>
+      </c>
+      <c r="H53" s="34"/>
+      <c r="I53" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E54" s="3">
+        <v>2</v>
+      </c>
+      <c r="F54" s="8">
+        <v>4</v>
+      </c>
+      <c r="G54" s="8">
+        <f>F54*E54</f>
+        <v>8</v>
+      </c>
+      <c r="H54" s="35"/>
+      <c r="I54" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="E55" s="3">
         <v>12</v>
       </c>
-      <c r="F48" s="14">
-        <v>5.9</v>
-      </c>
-      <c r="G48" s="14">
-        <f t="shared" si="0"/>
-        <v>70.800000000000011</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="I48" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="E49" s="3">
-        <v>8</v>
-      </c>
-      <c r="F49" s="14">
-        <v>45</v>
-      </c>
-      <c r="G49" s="14">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="H49" s="6" t="s">
+      <c r="F55" s="8">
+        <v>105.31</v>
+      </c>
+      <c r="G55" s="8">
+        <f>F55*E55</f>
+        <v>1263.72</v>
+      </c>
+      <c r="H55" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="I49" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B50" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="E50" s="3">
-        <v>1</v>
-      </c>
-      <c r="F50" s="14">
-        <v>7.2</v>
-      </c>
-      <c r="G50" s="14">
-        <f t="shared" si="0"/>
-        <v>7.2</v>
-      </c>
-      <c r="H50" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="I50" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="E51" s="3">
-        <v>2</v>
-      </c>
-      <c r="F51" s="14">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="G51" s="14">
-        <f t="shared" si="0"/>
-        <v>18.600000000000001</v>
-      </c>
-      <c r="H51" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="I51" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="E52" s="3">
-        <v>1</v>
-      </c>
-      <c r="F52" s="14">
-        <v>4</v>
-      </c>
-      <c r="G52" s="14">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H52" s="6"/>
-      <c r="I52" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="E53" s="3">
-        <v>2</v>
-      </c>
-      <c r="F53" s="14">
-        <v>4</v>
-      </c>
-      <c r="G53" s="14">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H53" s="7"/>
-      <c r="I53" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D54" s="12" t="s">
+      <c r="I55" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E54" s="3">
-        <v>12</v>
-      </c>
-      <c r="F54" s="14">
-        <v>105.31</v>
-      </c>
-      <c r="G54" s="14">
-        <f t="shared" si="0"/>
-        <v>1263.72</v>
-      </c>
-      <c r="H54" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="I54" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
+      <c r="B56" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="B55" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="E55" s="3">
-        <v>2</v>
-      </c>
-      <c r="F55" s="14">
-        <v>0.76</v>
-      </c>
-      <c r="G55" s="14">
-        <f t="shared" si="0"/>
-        <v>1.52</v>
-      </c>
-      <c r="H55" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="I55" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="B56" s="12" t="s">
-        <v>161</v>
-      </c>
       <c r="C56" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>160</v>
+        <v>65</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>157</v>
       </c>
       <c r="E56" s="3">
         <v>2</v>
       </c>
-      <c r="F56" s="14">
-        <v>6.5</v>
-      </c>
-      <c r="G56" s="14">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="H56" s="6" t="s">
-        <v>226</v>
+      <c r="F56" s="8">
+        <v>0.76</v>
+      </c>
+      <c r="G56" s="8">
+        <f>F56*E56</f>
+        <v>1.52</v>
+      </c>
+      <c r="H56" s="34" t="s">
+        <v>222</v>
       </c>
       <c r="I56" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B57" s="12" t="s">
-        <v>228</v>
+      <c r="A57" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D57" s="12" t="s">
-        <v>163</v>
+        <v>56</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>159</v>
       </c>
       <c r="E57" s="3">
         <v>2</v>
       </c>
-      <c r="F57" s="14">
+      <c r="F57" s="8">
+        <v>6.5</v>
+      </c>
+      <c r="G57" s="8">
+        <f>F57*E57</f>
+        <v>13</v>
+      </c>
+      <c r="H57" s="34" t="s">
+        <v>223</v>
+      </c>
+      <c r="I57" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E58" s="3">
+        <v>2</v>
+      </c>
+      <c r="F58" s="8">
         <v>230</v>
       </c>
-      <c r="G57" s="14">
-        <f t="shared" si="0"/>
+      <c r="G58" s="8">
+        <f>F58*E58</f>
         <v>460</v>
       </c>
-      <c r="H57" s="6" t="s">
+      <c r="H58" s="34" t="s">
+        <v>224</v>
+      </c>
+      <c r="I58" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="I57" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="B58" s="13" t="s">
-        <v>229</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="D58" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="E58" s="10">
+      <c r="D59" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E59" s="3">
         <v>4</v>
       </c>
-      <c r="F58" s="15">
+      <c r="F59" s="8">
         <v>8</v>
       </c>
-      <c r="G58" s="15">
-        <f t="shared" si="0"/>
+      <c r="G59" s="8">
+        <f>F59*E59</f>
         <v>32</v>
       </c>
-      <c r="H58" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="I58" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="2"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="16" t="s">
+      <c r="H59" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="I59" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D60" s="24" t="s">
         <v>234</v>
       </c>
-      <c r="G59" s="17">
-        <f>SUM(G2:G58)</f>
-        <v>6984.5000000000009</v>
-      </c>
-      <c r="I59" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="2"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
+      <c r="E60" s="25">
+        <v>1</v>
+      </c>
+      <c r="F60" s="26">
+        <v>14</v>
+      </c>
+      <c r="G60" s="26">
+        <f>F60*E60</f>
+        <v>14</v>
+      </c>
+      <c r="H60" s="36" t="s">
+        <v>235</v>
+      </c>
       <c r="I60" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="3"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
+      <c r="F61" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="G61" s="17">
+        <f>SUM(G2:G60)</f>
+        <v>6999.6</v>
+      </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I62" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I63" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="65" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I65" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -3144,23 +3226,25 @@
     <hyperlink ref="H40" r:id="rId38"/>
     <hyperlink ref="H41" r:id="rId39"/>
     <hyperlink ref="H42" r:id="rId40"/>
-    <hyperlink ref="H44" r:id="rId41"/>
-    <hyperlink ref="H45" r:id="rId42"/>
-    <hyperlink ref="H46" r:id="rId43"/>
-    <hyperlink ref="H47" r:id="rId44"/>
-    <hyperlink ref="H48" r:id="rId45"/>
-    <hyperlink ref="H49" r:id="rId46"/>
-    <hyperlink ref="H50" r:id="rId47"/>
-    <hyperlink ref="H51" r:id="rId48"/>
-    <hyperlink ref="H54" r:id="rId49"/>
-    <hyperlink ref="H55" r:id="rId50"/>
-    <hyperlink ref="H56" r:id="rId51"/>
-    <hyperlink ref="H57" r:id="rId52"/>
-    <hyperlink ref="H58" r:id="rId53"/>
-    <hyperlink ref="H43" r:id="rId54"/>
+    <hyperlink ref="H45" r:id="rId41"/>
+    <hyperlink ref="H46" r:id="rId42"/>
+    <hyperlink ref="H47" r:id="rId43"/>
+    <hyperlink ref="H48" r:id="rId44"/>
+    <hyperlink ref="H49" r:id="rId45"/>
+    <hyperlink ref="H50" r:id="rId46"/>
+    <hyperlink ref="H51" r:id="rId47"/>
+    <hyperlink ref="H52" r:id="rId48"/>
+    <hyperlink ref="H55" r:id="rId49"/>
+    <hyperlink ref="H56" r:id="rId50"/>
+    <hyperlink ref="H57" r:id="rId51"/>
+    <hyperlink ref="H58" r:id="rId52"/>
+    <hyperlink ref="H59" r:id="rId53"/>
+    <hyperlink ref="H44" r:id="rId54"/>
     <hyperlink ref="H25" r:id="rId55"/>
+    <hyperlink ref="H60" r:id="rId56"/>
+    <hyperlink ref="H43" r:id="rId57"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId56"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId58"/>
 </worksheet>
 </file>
</xml_diff>